<commit_message>
Fixed menu layout and added hide/open states for menu sections
</commit_message>
<xml_diff>
--- a/src/content/menu.xlsx
+++ b/src/content/menu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="246">
   <si>
     <t>order</t>
   </si>
@@ -716,15 +716,27 @@
     <t>Steamed Seafood Delight with Mixed Vegetables</t>
   </si>
   <si>
+    <t>All served with chicken fried with a side of either one egg roll or two crab rangoon.</t>
+  </si>
+  <si>
+    <t>All served with a side of white rice.</t>
+  </si>
+  <si>
+    <t>All served with chicken fried with a side of either one egg roll, two crab rangoon, or a cup of hot &amp; sour soup, egg drop soup, or wonton soup.</t>
+  </si>
+  <si>
+    <t>No salt, low calorie, and steamed dishes with a side of white rice and sauce separated on the side.</t>
+  </si>
+  <si>
+    <t>A party special is three quarts of a dish served on one big tray. This does not come with any rice.</t>
+  </si>
+  <si>
     <t>Pint sized soups come with one packet of fried crunchy noodles, while quart sizes come with two.</t>
   </si>
   <si>
     <t>All served with a side of white rice and a packet of fried crunchy noodles.</t>
   </si>
   <si>
-    <t>All served with a side of white rice.</t>
-  </si>
-  <si>
     <t>A soft and thick brown noodle.</t>
   </si>
   <si>
@@ -737,16 +749,7 @@
     <t>All served with a side of white rice and a cup of sweet &amp; sour sauce.</t>
   </si>
   <si>
-    <t>All served with chicken fried with a side of either one egg roll or two crab rangoon.</t>
-  </si>
-  <si>
     <t>All served with a side of white rice and a cup of egg foo young sauce.</t>
-  </si>
-  <si>
-    <t>A party special is three quarts of a dish served on one big tray. This does not come with any rice.</t>
-  </si>
-  <si>
-    <t>No salt, low calorie, and steamed dishes with a side of white rice and sauce separated on the side.</t>
   </si>
 </sst>
 </file>
@@ -783,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -797,6 +800,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -5186,7 +5190,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.14"/>
     <col customWidth="1" min="2" max="2" width="24.43"/>
-    <col customWidth="1" min="3" max="3" width="83.43"/>
+    <col customWidth="1" min="3" max="3" width="117.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5204,8 +5208,11 @@
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3">
@@ -5213,10 +5220,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>164</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="4">
@@ -5224,10 +5231,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>209</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5">
@@ -5235,10 +5242,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>236</v>
+        <v>223</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="6">
@@ -5246,183 +5253,180 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>201</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>6.0</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>237</v>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>7.0</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>238</v>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
         <v>8.0</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>236</v>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
         <v>9.0</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
         <v>10.0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>236</v>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
         <v>11.0</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>236</v>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>12.0</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>236</v>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
         <v>13.0</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>236</v>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
         <v>14.0</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>143</v>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
         <v>15.0</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>241</v>
+      <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
         <v>16.0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>236</v>
+      <c r="B17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
         <v>17.0</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>191</v>
+      <c r="B18" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
         <v>18.0</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>236</v>
+      <c r="B19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
         <v>19.0</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>201</v>
+      <c r="B20" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
         <v>20.0</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>241</v>
+      <c r="B21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
         <v>21.0</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>223</v>
+      <c r="B22" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>